<commit_message>
Implemented normalization algorithm (#24)
* Added normalize function

* Added new object 'NormalizedObject' for normalizing objects

* Added more functionality for normalizing the scores

* Minor changes

* Added more detections for confidence levels

* Adjusted confidence percentages for normalizer function

* Added pycache files

* Teeny adjustments
</commit_message>
<xml_diff>
--- a/docs/negative.xlsx
+++ b/docs/negative.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">the party scenes deliver some tawdry kicks . the rest of the film . . . is dudsville . </t>
   </si>
   <si>
-    <t xml:space="preserve">our culture is headed down the toilet with the ferocity of a frozen burrito after an all-night tequila bender � and i know this because i've seen 'jackass : the movie . '</t>
+    <t xml:space="preserve">our culture is headed down the toilet with the ferocity of a frozen burrito after an all-night tequila bender �and i know this because i've seen 'jackass : the movie . '</t>
   </si>
   <si>
     <t xml:space="preserve">the criticism never rises above easy , cynical potshots at morally bankrupt characters . . . </t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">somewhere in the middle , the film compels , as demme experiments he harvests a few movie moment gems , but the field of roughage dominates . </t>
   </si>
   <si>
-    <t xml:space="preserve">the action clich�s just pile up . </t>
+    <t xml:space="preserve">the action clich� just pile up . </t>
   </si>
   <si>
     <t xml:space="preserve">payami tries to raise some serious issues about iran's electoral process , but the result is a film that's about as subtle as a party political broadcast . </t>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">though her fans will assuredly have their funny bones tickled , others will find their humor-seeking dollars best spent elsewhere . </t>
   </si>
   <si>
-    <t xml:space="preserve">pascale bailly's rom-com provides am�lie's audrey tautou with another fabuleux destin -- i . e . , a banal spiritual quest . </t>
+    <t xml:space="preserve">pascale bailly's rom-com provides am�ie's audrey tautou with another fabuleux destin -- i . e . , a banal spiritual quest . </t>
   </si>
   <si>
     <t xml:space="preserve">a static and sugary little half-hour , after-school special about interfaith understanding , stretched out to 90 minutes . </t>
@@ -361,7 +361,7 @@
     <t xml:space="preserve">in the telling of a story largely untold , bui chooses to produce something that is ultimately suspiciously familiar . </t>
   </si>
   <si>
-    <t xml:space="preserve">the plot is nothing but boilerplate clich�s from start to finish , and the script assumes that not only would subtlety be lost on the target audience , but that it's also too stupid to realize that they've already seen this exact same movie a hundred times</t>
+    <t xml:space="preserve">the plot is nothing but boilerplate clich� from start to finish , and the script assumes that not only would subtlety be lost on the target audience , but that it's also too stupid to realize that they've already seen this exact same movie a hundred times</t>
   </si>
   <si>
     <t xml:space="preserve">terminally brain dead production . </t>
@@ -682,7 +682,7 @@
     <t xml:space="preserve">although disney follows its standard formula in this animated adventure , it feels more forced than usual . </t>
   </si>
   <si>
-    <t xml:space="preserve">gaghan . . . has thrown every suspenseful clich� in the book at this nonsensical story . </t>
+    <t xml:space="preserve">gaghan . . . has thrown every suspenseful clich�in the book at this nonsensical story . </t>
   </si>
   <si>
     <t xml:space="preserve">a sham construct based on theory , sleight-of-hand , and ill-wrought hypothesis . </t>
@@ -736,7 +736,7 @@
     <t xml:space="preserve">the film can depress you about life itself . </t>
   </si>
   <si>
-    <t xml:space="preserve">i'm sure the filmmakers found this a remarkable and novel concept , but anybody who has ever seen an independent film can report that it is instead a cheap clich� . </t>
+    <t xml:space="preserve">i'm sure the filmmakers found this a remarkable and novel concept , but anybody who has ever seen an independent film can report that it is instead a cheap clich�. </t>
   </si>
   <si>
     <t xml:space="preserve">the acting is fine but the script is about as interesting as a recording of conversations at the wal-mart checkout line . </t>
@@ -835,7 +835,7 @@
     <t xml:space="preserve">diane lane's sophisticated performance can't rescue adrian lyne's unfaithful from its sleazy moralizing . </t>
   </si>
   <si>
-    <t xml:space="preserve">not at all clear what it's trying to say and even if it were � i doubt it would be all that interesting . </t>
+    <t xml:space="preserve">not at all clear what it's trying to say and even if it were �i doubt it would be all that interesting . </t>
   </si>
   <si>
     <t xml:space="preserve">storytelling feels slight . </t>
@@ -1354,7 +1354,7 @@
     <t xml:space="preserve">there's a lot of good material here , but there's also a lot of redundancy and unsuccessful crudeness accompanying it . </t>
   </si>
   <si>
-    <t xml:space="preserve">absurdities and clich�s accumulate like lint in a fat man's navel . </t>
+    <t xml:space="preserve">absurdities and clich� accumulate like lint in a fat man's navel . </t>
   </si>
   <si>
     <t xml:space="preserve">if you think it's a riot to see rob schneider in a young woman's clothes , then you'll enjoy the hot chick . </t>
@@ -1396,7 +1396,7 @@
     <t xml:space="preserve">these two are generating about as much chemistry as an iraqi factory poised to receive a un inspector . </t>
   </si>
   <si>
-    <t xml:space="preserve">respons�vel direto pelo fracasso 'art�stico' de doce lar , o roteirista c . jay cox n�o consegue sequer aproveitar os pouqu�ssimos momentos em que escapa da mediocridade . </t>
+    <t xml:space="preserve">respons�el direto pelo fracasso 'art�tico' de doce lar , o roteirista c . jay cox n� consegue sequer aproveitar os pouqu�simos momentos em que escapa da mediocridade . </t>
   </si>
   <si>
     <t xml:space="preserve">just as the lousy tarantino imitations have subsided , here comes the first lousy guy ritchie imitation . </t>
@@ -1444,7 +1444,22 @@
     <t xml:space="preserve">alarms for duvall's throbbing sincerity and his elderly propensity for patting people while he talks . </t>
   </si>
   <si>
-    <t xml:space="preserve">�the maudlin way its story unfolds suggests a director fighting against the urge to sensationalize his material . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿻</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">he maudlin way its story unfolds suggests a director fighting against the urge to sensationalize his material . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">what little grace [rifkin's] tale of precarious skid-row dignity achieves is pushed into the margins by predictable plotting and tiresome histrionics . </t>
@@ -1582,7 +1597,7 @@
     <t xml:space="preserve">adults , other than the parents . . . will be hard pressed to succumb to the call of the wild . </t>
   </si>
   <si>
-    <t xml:space="preserve">brady achieves the remarkable feat of squandering a topnotch foursome of actors . . . by shoving them into every clich�d white-trash situation imaginable . </t>
+    <t xml:space="preserve">brady achieves the remarkable feat of squandering a topnotch foursome of actors . . . by shoving them into every clich� white-trash situation imaginable . </t>
   </si>
   <si>
     <t xml:space="preserve">in the name of an allegedly inspiring and easily marketable flick , the emperor's club turns a blind eye to the very history it pretends to teach . </t>
@@ -1594,7 +1609,7 @@
     <t xml:space="preserve">a direct-to-void release , heading nowhere . </t>
   </si>
   <si>
-    <t xml:space="preserve">typical anim� , with cheapo animation ( like saturday morning tv in the '60s ) , a complex sword-and-sorcery plot and characters who all have big round eyes and japanese names . </t>
+    <t xml:space="preserve">typical anim�, with cheapo animation ( like saturday morning tv in the '60s ) , a complex sword-and-sorcery plot and characters who all have big round eyes and japanese names . </t>
   </si>
   <si>
     <t xml:space="preserve">below is well below expectations . </t>
@@ -1927,7 +1942,30 @@
     <t xml:space="preserve">it's better than mid-range steven seagal , but not as sharp as jet li on rollerblades . </t>
   </si>
   <si>
-    <t xml:space="preserve">no dia em que aceitou dirigir esta continua��o , harold ramis deve ter sa�do da cama com o p� esquerdo . e aqueles que decidiram assistir a este filme tamb�m . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">no dia em que aceitou dirigir esta continua</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">豫</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">o , harold ramis deve ter sa�o da cama com o p�esquerdo . e aqueles que decidiram assistir a este filme tamb� . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">there's a reason why halftime is only fifteen minutes long . </t>
@@ -2071,7 +2109,7 @@
     <t xml:space="preserve">a well-made but emotionally scattered film whose hero gives his heart only to the dog . </t>
   </si>
   <si>
-    <t xml:space="preserve">the most repugnant adaptation of a classic text since roland joff� and demi moore's the scarlet letter . </t>
+    <t xml:space="preserve">the most repugnant adaptation of a classic text since roland joff�and demi moore's the scarlet letter . </t>
   </si>
   <si>
     <t xml:space="preserve">the isolated moments of creative insanity finally are lost in the thin soup of canned humor . </t>
@@ -2197,7 +2235,7 @@
     <t xml:space="preserve">one scene after another in this supposedly funny movie falls to the floor with a sickening thud . </t>
   </si>
   <si>
-    <t xml:space="preserve">'the ch�teau is never quite able to overcome the cultural moat surrounding its ludicrous and contrived plot . '</t>
+    <t xml:space="preserve">'the ch�eau is never quite able to overcome the cultural moat surrounding its ludicrous and contrived plot . '</t>
   </si>
   <si>
     <t xml:space="preserve">meyjes focuses too much on max when he should be filling the screen with this tortured , dull artist and monster-in-the- making . </t>
@@ -2344,7 +2382,7 @@
     <t xml:space="preserve">hill looks to be going through the motions , beginning with the pale script . </t>
   </si>
   <si>
-    <t xml:space="preserve">howard conjures the past via surrealist flourishes so overwrought you'd swear he just stepped out of a bu�uel retrospective . </t>
+    <t xml:space="preserve">howard conjures the past via surrealist flourishes so overwrought you'd swear he just stepped out of a bu�el retrospective . </t>
   </si>
   <si>
     <t xml:space="preserve">the best thing that can be said of the picture is that it does have a few cute moments . </t>
@@ -2395,7 +2433,7 @@
     <t xml:space="preserve">borstal boy represents the worst kind of filmmaking , the kind that pretends to be passionate and truthful but is really frustratingly timid and soggy . </t>
   </si>
   <si>
-    <t xml:space="preserve">the film's lack of personality permeates all its aspects � from the tv movie-esque , affected child acting to the dullest irish pub scenes ever filmed . </t>
+    <t xml:space="preserve">the film's lack of personality permeates all its aspects �from the tv movie-esque , affected child acting to the dullest irish pub scenes ever filmed . </t>
   </si>
   <si>
     <t xml:space="preserve">works on the whodunit level as its larger themes get lost in the murk of its own making</t>
@@ -2467,7 +2505,30 @@
     <t xml:space="preserve">the film feels formulaic , its plot and pacing typical hollywood war-movie stuff , while the performances elicit more of a sense of deja vu than awe . </t>
   </si>
   <si>
-    <t xml:space="preserve">this overproduced piece of dreck is shockingly bad and absolutely unnecessary . hmmm�might i suggest that the wayward wooden one end it all by stuffing himself into an electric pencil sharpener ? </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">this overproduced piece of dreck is shockingly bad and absolutely unnecessary . hmmm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ight i suggest that the wayward wooden one end it all by stuffing himself into an electric pencil sharpener ? </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">the makers of mothman prophecies succeed in producing that most frightening of all movies -- a mediocre horror film too bad to be good and too good to be bad . </t>
@@ -2602,7 +2663,7 @@
     <t xml:space="preserve">reggio and glass so rhapsodize cynicism , with repetition and languorous slo-mo sequences , that glass's dirgelike score becomes a fang-baring lullaby . </t>
   </si>
   <si>
-    <t xml:space="preserve">es triste tener que decirles que lo �nico grato de la cinta es el cuerpo desnudo de la heather . . . </t>
+    <t xml:space="preserve">es triste tener que decirles que lo �ico grato de la cinta es el cuerpo desnudo de la heather . . . </t>
   </si>
   <si>
     <t xml:space="preserve">ends up offering nothing more than the latest schwarzenegger or stallone flick would . </t>
@@ -2899,7 +2960,7 @@
     <t xml:space="preserve">a simpler , leaner treatment would have been preferable ; after all , being about nothing is sometimes funnier than being about something . </t>
   </si>
   <si>
-    <t xml:space="preserve">the characters are based on stock clich�s , and the attempt to complicate the story only defies credibility . </t>
+    <t xml:space="preserve">the characters are based on stock clich� , and the attempt to complicate the story only defies credibility . </t>
   </si>
   <si>
     <t xml:space="preserve">everything about it from the bland songs to the colorful but flat drawings is completely serviceable and quickly forgettable . </t>
@@ -3218,7 +3279,13 @@
     <t xml:space="preserve">the director mostly plays it straight , turning leys' fable into a listless climb down the social ladder . </t>
   </si>
   <si>
-    <t xml:space="preserve"> bad " is the operative word for " bad company , " and i don't mean that in a good way . 
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bad " is the operative word for " bad company , " and i don't mean that in a good way . 
 though frida is easier to swallow than julie taymor's preposterous titus , the eye candy here lacks considerable brio . 
 drumline is -- the mere suggestion , albeit a visually compelling one , of a fully realized story . 
 the whole movie is simply a lazy exercise in bad filmmaking that asks you to not only suspend your disbelief but your intelligence as well . 
@@ -3228,14 +3295,14 @@
 it's loud and boring ; watching it is like being trapped at a bad rock concert . 
 merely ( and literally ) tosses around sex toys and offers half-hearted paeans to empowerment that are repeatedly undercut by the brutality of the jokes , most at women's expense . 
 if you want a movie time trip , the 1960 version is a far smoother ride . 
-traffics in the kind of prechewed racial clich�s that have already been through the corporate stand-up-comedy mill . 
+traffics in the kind of prechewed racial clich� that have already been through the corporate stand-up-comedy mill . 
 the story is -- forgive me -- a little thin , and the filmmaking clumsy and rushed . 
  . . . grows decidedly flimsier with its many out-sized , out of character and logically porous action set pieces . 
 i wish windtalkers had had more faith in the dramatic potential of this true story . this would have been better than the fiction it has concocted , and there still could have been room for the war scenes . 
 aggressive self-glorification and a manipulative whitewash . stay for the credits and see a devastating comic impersonation by dustin hoffman that is revelatory . 
 none of the characters or plot-lines are fleshed-out enough to build any interest . 
-as social expos� , skins has its heart in the right place , but that's not much to hang a soap opera on . 
-the whole film has this sneaky feel to it � as if the director is trying to dupe the viewer into taking it all as very important simply because the movie is ugly to look at and not a hollywood product . 
+as social expos�, skins has its heart in the right place , but that's not much to hang a soap opera on . 
+the whole film has this sneaky feel to it �as if the director is trying to dupe the viewer into taking it all as very important simply because the movie is ugly to look at and not a hollywood product . 
 there's a bit of thematic meat on the bones of queen of the damned , as its origins in an anne rice novel dictate , but generally , it's a movie that emphasizes style over character and substance . 
 the only way to tolerate this insipid , brutally clueless film might be with a large dose of painkillers . 
 this one is certainly well-meaning , but it's also simple-minded and contrived . 
@@ -3271,7 +3338,7 @@
 large budget notwithstanding , the movie is such a blip on the year's radar screen that it's tempting just to go with it for the ride . but this time , the old mib label stands for milder isn't better . 
 feels familiar and tired . 
 a retread of material already thoroughly plumbed by martin scorsese . 
-instead of making his own style , director marcus adams just copies from various sources � good sources , bad mixture
+instead of making his own style , director marcus adams just copies from various sources �good sources , bad mixture
 criminal conspiracies and true romances move so easily across racial and cultural lines in the film that it makes my big fat greek wedding look like an apartheid drama . 
 a bore that tends to hammer home every one of its points . 
 a story which fails to rise above its disgusting source material . 
@@ -3297,14 +3364,46 @@
 doesn't get the job done , running off the limited chemistry created by ralph fiennes and jennifer lopez . 
 a particularly joyless , and exceedingly dull , period coming-of-age tale . 
 it's impossible to indulge the fanciful daydreams of janice beard ( eileen walsh ) when her real-life persona is so charmless and vacant . 
-�it wasn't the subject matter that ultimately defeated the film�it was the unfulfilling , incongruous , " wait a second , did i miss something ? " ending . 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">t wasn't the subject matter that ultimately defeated the film</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">t was the unfulfilling , incongruous , " wait a second , did i miss something ? " ending . 
 this is a movie where the most notable observation is how long you've been sitting still . 
 poor editing , bad bluescreen , and ultra-cheesy dialogue highlight the radical action . 
 it's super- violent , super-serious and super-stupid . 
 so earnest and well-meaning , and so stocked with talent , that you almost forget the sheer , ponderous awfulness of its script . 
 just a string of stale gags , with no good inside dope , and no particular bite . 
 it's splash without the jokes . 
-the ch�teau would have been benefited from a sharper , cleaner script before it went in front of the camera . not to mention a sharper , cleaner camera lens . 
+the ch�eau would have been benefited from a sharper , cleaner script before it went in front of the camera . not to mention a sharper , cleaner camera lens . 
 shallow , noisy and pretentious . 
 morrissette has performed a difficult task indeed - he's taken one of the world's most fascinating stories and made it dull , lifeless , and irritating . 
 granddad of le nouvelle vague , jean-luc godard continues to baffle the faithful with his games of hide-and-seek . 
@@ -3343,6 +3442,7 @@
  " what john does is heroic , but we don't condone it , " one of the film's stars recently said , a tortuous comment that perfectly illustrates the picture's moral schizophrenia . 
 like coming into a long-running , well-written television series where you've missed the first half-dozen episodes and probably won't see the next six . 
 this is no " waterboy !  </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">its generic villains lack any intrigue ( other than their funny accents ) and the action scenes are poorly delivered . </t>
@@ -3633,7 +3733,7 @@
     <t xml:space="preserve">when not wallowing in its characters' frustrations , the movie is busy contriving false , sitcom-worthy solutions to their problems . </t>
   </si>
   <si>
-    <t xml:space="preserve">an overstylized , pur�ed m�lange of sex , psychology , drugs and philosophy . sometimes entertaining , sometimes indulgent -- but never less than pure wankery . </t>
+    <t xml:space="preserve">an overstylized , pur�d m�ange of sex , psychology , drugs and philosophy . sometimes entertaining , sometimes indulgent -- but never less than pure wankery . </t>
   </si>
   <si>
     <t xml:space="preserve">'lovely and amazing , ' unhappily , is neither . . . excessively strained and contrived . </t>
@@ -3687,7 +3787,7 @@
     <t xml:space="preserve">extremely bad . </t>
   </si>
   <si>
-    <t xml:space="preserve">a clich�d and shallow cautionary tale about the hard-partying lives of gay men . </t>
+    <t xml:space="preserve">a clich� and shallow cautionary tale about the hard-partying lives of gay men . </t>
   </si>
   <si>
     <t xml:space="preserve">the fetid underbelly of fame has never looked uglier . </t>
@@ -4005,7 +4105,7 @@
     <t xml:space="preserve">cassavetes thinks he's making dog day afternoon with a cause , but all he's done is to reduce everything he touches to a shrill , didactic cartoon . </t>
   </si>
   <si>
-    <t xml:space="preserve">buries an interesting storyline about morality and the choices we make underneath such a mountain of clich�s and borrowed images that it might more accurately be titled mr . chips off the old block . </t>
+    <t xml:space="preserve">buries an interesting storyline about morality and the choices we make underneath such a mountain of clich� and borrowed images that it might more accurately be titled mr . chips off the old block . </t>
   </si>
   <si>
     <t xml:space="preserve">although sensitive to a fault , it's often overwritten , with a surfeit of weighty revelations , flowery dialogue , and nostalgia for the past and roads not taken . </t>
@@ -4014,7 +4114,7 @@
     <t xml:space="preserve">it's so badly made on every level that i'm actually having a hard time believing people were paid to make it . </t>
   </si>
   <si>
-    <t xml:space="preserve">without non-stop techno or the existential overtones of a kieslowski morality tale , maelstr�m is just another winter sleepers . </t>
+    <t xml:space="preserve">without non-stop techno or the existential overtones of a kieslowski morality tale , maelstr� is just another winter sleepers . </t>
   </si>
   <si>
     <t xml:space="preserve">nicks , seemingly uncertain what's going to make people laugh , runs the gamut from stale parody to raunchy sex gags to formula romantic comedy . </t>
@@ -4143,7 +4243,7 @@
     <t xml:space="preserve">even with a green mohawk and a sheet of fire-red flame tattoos covering his shoulder , however , kilmer seems to be posing , rather than acting . and that leaves a hole in the center of the salton sea . </t>
   </si>
   <si>
-    <t xml:space="preserve">there's just no currency in deriding james bond for being a clich�d , doddering , misogynistic boy's club . </t>
+    <t xml:space="preserve">there's just no currency in deriding james bond for being a clich� , doddering , misogynistic boy's club . </t>
   </si>
   <si>
     <t xml:space="preserve">when the film ended , i felt tired and drained and wanted to lie on my own deathbed for a while . </t>
@@ -4179,7 +4279,7 @@
     <t xml:space="preserve">rarely has leukemia looked so shimmering and benign . </t>
   </si>
   <si>
-    <t xml:space="preserve">� is an arthritic attempt at directing by callie khouri . i had to look away - this was god awful . </t>
+    <t xml:space="preserve">�is an arthritic attempt at directing by callie khouri . i had to look away - this was god awful . </t>
   </si>
   <si>
     <t xml:space="preserve">even in this less-than-magic kingdom , reese rules . </t>
@@ -4320,7 +4420,7 @@
     <t xml:space="preserve">almost gags on its own gore . </t>
   </si>
   <si>
-    <t xml:space="preserve">how do you spell clich� ? </t>
+    <t xml:space="preserve">how do you spell clich�? </t>
   </si>
   <si>
     <t xml:space="preserve">it's sweet , harmless , dumb , occasionally funny and about as compelling as a fishing show . </t>
@@ -4332,7 +4432,7 @@
     <t xml:space="preserve">while [hill] has learned new tricks , the tricks alone are not enough to salvage this lifeless boxing film . </t>
   </si>
   <si>
-    <t xml:space="preserve">in the real world , an actor this uncharismatically beautiful would have a r�sum� loaded with credits like " girl in bar #3 . " </t>
+    <t xml:space="preserve">in the real world , an actor this uncharismatically beautiful would have a r�um�loaded with credits like " girl in bar #3 . " </t>
   </si>
   <si>
     <t xml:space="preserve">too much of it feels unfocused and underdeveloped . </t>
@@ -4686,7 +4786,29 @@
     <t xml:space="preserve">it's one of those baseball pictures where the hero is stoic , the wife is patient , the kids are as cute as all get-out and the odds against success are long enough to intimidate , but short enough to make a dream seem possible . </t>
   </si>
   <si>
-    <t xml:space="preserve"> the time machine " is a movie that has no interest in itself . it doesn't believe in itself , it has no sense of humor�it's just plain bored . 
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> the time machine " is a movie that has no interest in itself . it doesn't believe in itself , it has no sense of humor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">t's just plain bored . 
  . . . a hollow joke told by a cinematic gymnast having too much fun embellishing the misanthropic tale to actually engage it . 
 a morose little soap opera about three vapid , insensitive people who take turns hurting each other . it's a feature-length adaptation of one of those " can this marriage be saved ? " columns from ladies home journal . . . 
 the film's essentially over by the meet-cute . 
@@ -4755,7 +4877,7 @@
 feels haphazard , as if the writers mistakenly thought they could achieve an air of frantic spontaneity by simply tossing in lots of characters doing silly stuff and stirring the pot . 
 what an embarrassment . 
 for each chuckle there are at least 10 complete misses , many coming from the amazingly lifelike tara reid , whose acting skills are comparable to a cardboard cutout . 
-in its own way , joshua is as blasphemous and nonsensical as a luis bu�uel film without the latter's attendant intelligence , poetry , passion , and genius . 
+in its own way , joshua is as blasphemous and nonsensical as a luis bu�el film without the latter's attendant intelligence , poetry , passion , and genius . 
 i've always dreamed of attending cannes , but after seeing this film , it's not that big a deal . 
 the vintage is pure '87 , with a halfhearted twist on its cautionary message : fatal attraction = don't have an affair with a nutjob ; unfaithful = don't if you're married to one . 
 a workshop mentality prevails . 
@@ -4796,9 +4918,9 @@
 i still can't relate to stuart : he's a mouse , for cryin' out loud , and all he does is milk it with despondent eyes and whine that nobody treats him human enough . 
 [serry] wants to blend politics and drama , an admirable ambition . it's too bad that the helping hand he uses to stir his ingredients is also a heavy one . 
 by the miserable standards to which the slasher genre has sunk , . . . actually pretty good . of course , by more objective measurements it's still quite bad . 
-the only entertainment you'll derive from this choppy and sloppy affair will be from unintentional giggles � several of them . 
+the only entertainment you'll derive from this choppy and sloppy affair will be from unintentional giggles �several of them . 
 sam mendes has become valedictorian at the school for soft landings and easy ways out . 
-l�stima por schwarzenegger , pero es hora de que deje la estafeta a las nuevas generaciones . 
+l�tima por schwarzenegger , pero es hora de que deje la estafeta a las nuevas generaciones . 
 exactly what it claims to be -- a simple diversion for the kids . 
 its story may be a thousand years old , but why did it have to seem like it took another thousand to tell it to us ? 
 woefully pretentious . 
@@ -4825,7 +4947,7 @@
 the film's tone and pacing are off almost from the get-go . 
 the talented and clever robert rodriguez perhaps put a little too much heart into his first film and didn't reserve enough for his second . 
 more whiny downer than corruscating commentary . 
-tambor and clayburgh make an appealing couple � he's understated and sardonic , she's appealingly manic and energetic . both deserve better . 
+tambor and clayburgh make an appealing couple �he's understated and sardonic , she's appealingly manic and energetic . both deserve better . 
 suffocated by its fussy script and uptight characters , this musty adaptation is all the more annoying since it's been packaged and sold back to us by hollywood . 
 coughs and sputters on its own postmodern conceit . 
 a wildly inconsistent emotional experience . 
@@ -4953,7 +5075,7 @@
 nothing in waking up in reno ever inspired me to think of its inhabitants as anything more than markers in a screenplay . 
 i'm just too bored to care . 
 irwin is a man with enough charisma and audacity to carry a dozen films , but this particular result is ultimately held back from being something greater . 
-not a stereotype is omitted nor a clich� left unsaid . 
+not a stereotype is omitted nor a clich�left unsaid . 
 as befits its title , this pg-13-rated piffle is ultimately as threatening as the snuggle fabric softener bear . 
 attempts by this ensemble film to impart a message are so heavy-handed that they instead pummel the audience . 
 it all feels like a monty python sketch gone horribly wrong . 
@@ -4973,7 +5095,8 @@
 the film tries too hard to be funny and tries too hard to be hip . the end result is a film that's neither . 
 every nanosecond of the the new guy reminds you that you could be doing something else far more pleasurable . something like scrubbing the toilet . or emptying rat traps . or doing last year's taxes with your ex-wife . 
 scooby dooby doo / and shaggy too / you both look and sound great . / but daphne , you're too buff / fred thinks he's tough / and velma - wow , you've lost weight ! 
-is the time really ri</t>
+is the time really ripe for</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">the subject of swinging still seems ripe for a documentary -- just not this one . </t>
@@ -5270,7 +5393,7 @@
     <t xml:space="preserve">expect to be reminded of other , better films , especially seven , which director william malone slavishly copies . </t>
   </si>
   <si>
-    <t xml:space="preserve">nair stuffs the film with dancing , henna , ornamentation , and group song , but her narrative clich�s and telegraphed episodes smell of old soap opera . </t>
+    <t xml:space="preserve">nair stuffs the film with dancing , henna , ornamentation , and group song , but her narrative clich� and telegraphed episodes smell of old soap opera . </t>
   </si>
   <si>
     <t xml:space="preserve">it's getting harder and harder to ignore the fact that hollywood isn't laughing with us , folks . it's laughing at us . </t>
@@ -5441,7 +5564,30 @@
     <t xml:space="preserve">the appeal of the vulgar , sexist , racist humour went over my head or -- considering just how low brow it is -- perhaps it snuck under my feet . </t>
   </si>
   <si>
-    <t xml:space="preserve">the story really has no place to go since simone is not real�she can't provide any conflict . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">the story really has no place to go since simone is not real</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">뾱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">he can't provide any conflict . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ihops don't pile on this much syrup . </t>
@@ -5501,7 +5647,7 @@
     <t xml:space="preserve">[i]f you've been to more than one indie flick in your life , chances are you've already seen this kind of thing . </t>
   </si>
   <si>
-    <t xml:space="preserve">first-time director jo�o pedro rodrigues' unwillingness to define his hero's background or motivations becomes more and more frustrating as the film goes on . </t>
+    <t xml:space="preserve">first-time director jo� pedro rodrigues' unwillingness to define his hero's background or motivations becomes more and more frustrating as the film goes on . </t>
   </si>
   <si>
     <t xml:space="preserve">no reason for anyone to invest their hard-earned bucks into a movie which obviously didn't invest much into itself either . </t>
@@ -5513,7 +5659,7 @@
     <t xml:space="preserve">a boring , wincingly cute and nauseatingly politically correct cartoon guaranteed to drive anyone much over age 4 screaming from the theater . </t>
   </si>
   <si>
-    <t xml:space="preserve">the vampire thriller blade ii starts off as a wild hoot and then sucks the blood out of its fun � toward the end , you can feel your veins cringing from the workout . </t>
+    <t xml:space="preserve">the vampire thriller blade ii starts off as a wild hoot and then sucks the blood out of its fun �toward the end , you can feel your veins cringing from the workout . </t>
   </si>
   <si>
     <t xml:space="preserve">when the first few villians are introduced as " spider " and " snake " you know you're in for a real winner , creativity at its peak . </t>
@@ -5624,7 +5770,7 @@
     <t xml:space="preserve">neither funny nor suspenseful nor particularly well-drawn . </t>
   </si>
   <si>
-    <t xml:space="preserve">'carente de imaginaci�n , mal dirigida , peor actuada y sin un �pice de romance , es una verdadera p�rdida de tiempo y dinero'</t>
+    <t xml:space="preserve">'carente de imaginaci� , mal dirigida , peor actuada y sin un �ice de romance , es una verdadera p�dida de tiempo y dinero'</t>
   </si>
   <si>
     <t xml:space="preserve">acting , particularly by tambor , almost makes " never again " worthwhile , but [writer/director] schaeffer should follow his titular advice</t>
@@ -5633,7 +5779,7 @@
     <t xml:space="preserve">both stars manage to be funny , but , like the recent i spy , the star chemistry begs the question of whether random gags add up to a movie . </t>
   </si>
   <si>
-    <t xml:space="preserve"> collateral damage " goes by the numbers and reps decent action entertainment � until the silly showdown ending that forces the viewer to totally suspend disbelief
+    <t xml:space="preserve"> collateral damage " goes by the numbers and reps decent action entertainment �until the silly showdown ending that forces the viewer to totally suspend disbelief
 'enigma' is a good name for a movie this delibrately obtuse and unapproachable . a waste of good performances . 
 a dreary , incoherent , self-indulgent mess of a movie in which a bunch of pompous windbags drone on inanely for two hours . . . a cacophony of pretentious , meaningless prattle . 
 i kept thinking over and over again , 'i should be enjoying this . ' but i wasn't . 
@@ -5746,7 +5892,7 @@
 this isn't just the cliffsnotes version of nicholas nickleby , it's the cliffsnotes with pages missing . 
 considering the harsh locations and demanding stunts , this must have been a difficult shoot , but the movie proves rough going for the audience as well . 
 better at putting you to sleep than a sound machine . 
-so clich�d that , at one point , they literally upset an apple cart . 
+so clich� that , at one point , they literally upset an apple cart . 
 it's a decent glimpse into a time period , and an outcast , that is no longer accessible , but it doesn't necessarily shed more light on its subject than the popular predecessor . 
 it might be the first sci-fi comedy that could benefit from a three's company-style laugh track . 
 when the plot kicks in , the film loses credibility . 
@@ -6048,7 +6194,22 @@
     <t xml:space="preserve">good for a few unintentional laughs , " extreme ops " was obviously made for the " xxx " crowd , people who enjoy mindless action without the benefit of decent acting , writing , and direction . </t>
   </si>
   <si>
-    <t xml:space="preserve">�a big , baggy , sprawling carnival of a movie , stretching out before us with little rhyme or reason . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿢 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">big , baggy , sprawling carnival of a movie , stretching out before us with little rhyme or reason . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">a frustrating combination of strained humor and heavy-handed sentimentality . </t>
@@ -6207,13 +6368,13 @@
     <t xml:space="preserve">a trashy , exploitative , thoroughly unpleasant experience . </t>
   </si>
   <si>
-    <t xml:space="preserve">newcomer helmer kevin donovan is hamstrung by a badly handled screenplay of what is really an amusing concept � a high-tech tux that transforms its wearer into a superman . </t>
+    <t xml:space="preserve">newcomer helmer kevin donovan is hamstrung by a badly handled screenplay of what is really an amusing concept �a high-tech tux that transforms its wearer into a superman . </t>
   </si>
   <si>
     <t xml:space="preserve">shouldn't have been allowed to use the word " new " in its title , because there's not an original character , siuation or joke in the entire movie . </t>
   </si>
   <si>
-    <t xml:space="preserve">often silly � and gross � but it's rarely as moronic as some campus gross-out films . </t>
+    <t xml:space="preserve">often silly �and gross �but it's rarely as moronic as some campus gross-out films . </t>
   </si>
   <si>
     <t xml:space="preserve">the advantage of a postapocalyptic setting is that it can be made on the cheap . any rock pile will do for a set . reign of fire has the disadvantage of also looking cheap . </t>
@@ -6291,7 +6452,7 @@
     <t xml:space="preserve">the story itself is uninteresting , and the songs are painfully undistinguished : they might be giants' so to be one of us may be the most tuneless tune ever composed . </t>
   </si>
   <si>
-    <t xml:space="preserve">este � apenas mais um ( longo ) epis�dio do programa da mtv . a �nica diferen�a � que , desta vez , a paramount teve o mau gosto de exibi-lo nos cinemas . </t>
+    <t xml:space="preserve">este �apenas mais um ( longo ) epis�io do programa da mtv . a �ica diferen� �que , desta vez , a paramount teve o mau gosto de exibi-lo nos cinemas . </t>
   </si>
   <si>
     <t xml:space="preserve">technically , the film is about as interesting as an insurance commercial . </t>
@@ -6523,7 +6684,7 @@
 after seeing swept away , i feel sorry for madonna . 
 instead of kicking off the intrigue and suspense and mystery of the whole thing , hart's war , like the st . louis rams in the super bowl , waits until after halftime to get started . 
 two-bit potboiler . 
-a gob of drivel so sickly sweet , even the eager consumers of moore's pasteurized ditties will retch it up like rancid cr�me br�l�e . 
+a gob of drivel so sickly sweet , even the eager consumers of moore's pasteurized ditties will retch it up like rancid cr�e br�� . 
 maudlin and melodramatic we expected . boring we didn't . 
 never quite transcends jokester status . . . and the punchline doesn't live up to barry's dead-eyed , perfectly chilled delivery . 
 the film's bathos often overwhelms what could have been a more multifaceted look at this interesting time and place . 
@@ -6541,7 +6702,7 @@
 if i spy were funny ( enough ) or exciting ( enough ) then it would be fairly simple to forgive the financial extortion it's trying to reap from the moviegoing public . 
 frustratingly , dridi tells us nothing about el gallo other than what emerges through his music . 
 places a slightly believable love triangle in a difficult-to-swallow setting , and then disappointingly moves the story into the realm of an improbable thriller . 
-stephen earnhart's documentary is a decomposition of healthy eccentric inspiration and ambition � wearing a cloak of unsentimental , straightforward text � when it's really an exercise in gross romanticization of the delusional personality type . 
+stephen earnhart's documentary is a decomposition of healthy eccentric inspiration and ambition �wearing a cloak of unsentimental , straightforward text �when it's really an exercise in gross romanticization of the delusional personality type . 
 a very average science fiction film . 
 undone by its overly complicated and derivative screenplay , the glacier-paced direction and the stereotypical characters . 
 how anyone over the age of 2 can stomach the touchy-feely message this preachy produce promotes is beyond us . 
@@ -6555,7 +6716,7 @@
 as with too many studio pics , plot mechanics get in the way of what should be the lighter-than-air adventure . 
 static , repetitive , muddy and blurry , hey arnold ! would seem to have a lock on the title of ugliest movie of the year . 
 for all of the contemporary post-colonialist consciousness that kapur tries to bring to the four feathers , the oddest thing about the movie is how it winds up affirming the same damn moldy values the material has always held dear . 
-un thriller manqu� qui tombe sur les nerfs presque d�s la premi�re image . 
+un thriller manqu�qui tombe sur les nerfs presque d� la premi�e image . 
 when it comes to entertainment , children deserve better than pokemon 4ever . 
 what the four feathers lacks is genuine sweep or feeling or even a character worth caring about . 
 while benigni ( who stars and co-wrote ) seems to be having a wonderful time , he might be alone in that . 
@@ -6685,7 +6846,7 @@
 the film equivalent of a toy chest whose contents get scattered over the course of 80 minutes . 
 just a bloody mess . 
 creepy but ultimately unsatisfying thriller . 
-martin scorsese cria um espet�culo visual que n�o possui alma - um filme esteticamente belo , mas emocionalmente frio . 
+martin scorsese cria um espet�ulo visual que n� possui alma - um filme esteticamente belo , mas emocionalmente frio . 
 you would be better off investing in the worthy emi recording that serves as the soundtrack , or the home video of the 1992 malfitano-domingo production . 
 has something to say . . . but it is a statement and issue worthy of a much more thoughtfulness and insight than a melodramatic and wholly predictable thriller . 
 bears is bad . not 'terrible filmmaking' bad , but more like , 'i once had a nightmare like this , and it's now coming true' bad . 
@@ -6726,7 +6887,7 @@
 it's so full of wrong choices that all you can do is shake your head in disbelief -- and worry about what classic oliver parker intends to mangle next time . 
 showtime is closer to slowtime . 
 it may be an easy swipe to take , but this barbershop just doesn't make the cut . 
-the weigh</t>
+the weight of water</t>
   </si>
   <si>
     <t xml:space="preserve">pryor lite , with half the demons , half the daring , much less talent , many fewer laughs . </t>
@@ -6762,10 +6923,33 @@
     <t xml:space="preserve">rainy days and movies about the disintegration of families always get me down . </t>
   </si>
   <si>
-    <t xml:space="preserve"> . . . has about 3/4th the fun of its spry 2001 predecessor � but it's a rushed , slapdash , sequel-for-the-sake- of-a-sequel with less than half the plot and ingenuity . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a incompet�ncia de marcus adams como roteirista s� � superada por sua p�ssima dire��o . </t>
+    <t xml:space="preserve"> . . . has about 3/4th the fun of its spry 2001 predecessor �but it's a rushed , slapdash , sequel-for-the-sake- of-a-sequel with less than half the plot and ingenuity . </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">a incompet�cia de marcus adams como roteirista s��superada por sua p�sima dire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">豫</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">o . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">the master of disaster - it's a piece of dreck disguised as comedy . </t>
@@ -6774,7 +6958,7 @@
     <t xml:space="preserve">this isn't a movie ; it's a symptom . </t>
   </si>
   <si>
-    <t xml:space="preserve">the film has a few cute ideas and several modest chuckles but it isn't exactly kiddie-friendly� alas , santa is more ho-hum than ho-ho-ho and the snowman ( who never gets to play that flute ) has all the charm of a meltdown . </t>
+    <t xml:space="preserve">the film has a few cute ideas and several modest chuckles but it isn't exactly kiddie-friendly�alas , santa is more ho-hum than ho-ho-ho and the snowman ( who never gets to play that flute ) has all the charm of a meltdown . </t>
   </si>
   <si>
     <t xml:space="preserve">the stupidest , most insulting movie of 2002's first quarter . </t>
@@ -7227,7 +7411,7 @@
     <t xml:space="preserve">the troubling thing about clockstoppers is that it doesn't make any sense . </t>
   </si>
   <si>
-    <t xml:space="preserve">with its paint fights , motorized scooter chases and dewy-eyed sentiment , it's a pretty listless collection of kid-movie clich�s . </t>
+    <t xml:space="preserve">with its paint fights , motorized scooter chases and dewy-eyed sentiment , it's a pretty listless collection of kid-movie clich� . </t>
   </si>
   <si>
     <t xml:space="preserve">mostly the film is just hectic and homiletic : two parts exhausting men in black mayhem to one part family values . </t>
@@ -7344,7 +7528,7 @@
     <t xml:space="preserve">as it stands it's an opera movie for the buffs . </t>
   </si>
   <si>
-    <t xml:space="preserve">la cinta comienza intentando ser un drama , r�pidamente se transforma en una comedia y termina por ser una parodia absolutamente predecible</t>
+    <t xml:space="preserve">la cinta comienza intentando ser un drama , r�idamente se transforma en una comedia y termina por ser una parodia absolutamente predecible</t>
   </si>
   <si>
     <t xml:space="preserve">this franchise has not spawned a single good film . the crap continues . </t>
@@ -7605,7 +7789,7 @@
     <t xml:space="preserve">to work , love stories require the full emotional involvement and support of a viewer . that is made almost impossible by events that set the plot in motion . </t>
   </si>
   <si>
-    <t xml:space="preserve">although barbershop boasts some of today's hottest and hippest acts from the world of television , music and stand-up comedy , this movie strangely enough has the outdated swagger of a shameless �70s blaxploitation shuck-and-jive sitcom . </t>
+    <t xml:space="preserve">although barbershop boasts some of today's hottest and hippest acts from the world of television , music and stand-up comedy , this movie strangely enough has the outdated swagger of a shameless �0s blaxploitation shuck-and-jive sitcom . </t>
   </si>
   <si>
     <t xml:space="preserve">a puzzle whose pieces do not fit . some are fascinating and others are not , and in the end , it is almost a good movie . </t>
@@ -7681,7 +7865,7 @@
 trailer trash cinema so uncool the only thing missing is the " gadzooks !  </t>
   </si>
   <si>
-    <t xml:space="preserve">her film is like a beautiful food entr�e that isn't heated properly , so that it ends up a bit cold and relatively flavorless . </t>
+    <t xml:space="preserve">her film is like a beautiful food entr� that isn't heated properly , so that it ends up a bit cold and relatively flavorless . </t>
   </si>
   <si>
     <t xml:space="preserve">like the world of his film , hartley created a monster but didn't know how to handle it . </t>
@@ -7747,7 +7931,7 @@
     <t xml:space="preserve">everything was as superficial as the forced new jersey lowbrow accent uma had . </t>
   </si>
   <si>
-    <t xml:space="preserve">o �timo esfor�o do diretor acaba sendo frustrado pelo roteiro , que , depois de levar um bom tempo para colocar a trama em andamento , perde-se de vez a partir do instante em que os estranhos acontecimentos s�o explicados . </t>
+    <t xml:space="preserve">o �imo esfor� do diretor acaba sendo frustrado pelo roteiro , que , depois de levar um bom tempo para colocar a trama em andamento , perde-se de vez a partir do instante em que os estranhos acontecimentos s� explicados . </t>
   </si>
   <si>
     <t xml:space="preserve">director david fincher and writer david koepp can't sustain it . </t>
@@ -7831,7 +8015,7 @@
     <t xml:space="preserve">lazily directed by charles stone iii . . . from a leaden script by matthew cirulnick and novelist thulani davis . </t>
   </si>
   <si>
-    <t xml:space="preserve">though jones and snipes are enthralling , the movie bogs down in rhetoric and clich� . </t>
+    <t xml:space="preserve">though jones and snipes are enthralling , the movie bogs down in rhetoric and clich�. </t>
   </si>
   <si>
     <t xml:space="preserve">the most remarkable ( and frustrating ) thing about world traveler , which opens today in manhattan , is that its protagonist , after being an object of intense scrutiny for 104 minutes , remains a complete blank . </t>
@@ -7900,7 +8084,7 @@
     <t xml:space="preserve">after sitting through this sloppy , made-for-movie comedy special , it makes me wonder if lawrence hates criticism so much that he refuses to evaluate his own work . </t>
   </si>
   <si>
-    <t xml:space="preserve">contrived pastiche of caper clich�s . </t>
+    <t xml:space="preserve">contrived pastiche of caper clich� . </t>
   </si>
   <si>
     <t xml:space="preserve">many shallower movies these days seem too long , but this one is egregiously short . </t>
@@ -7924,7 +8108,30 @@
     <t xml:space="preserve">loud , chaotic and largely unfunny . </t>
   </si>
   <si>
-    <t xml:space="preserve">i can't remember the last time i saw an audience laugh so much during a movie , but there's only one problem�it's supposed to be a drama . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">i can't remember the last time i saw an audience laugh so much during a movie , but there's only one problem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">t's supposed to be a drama . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">qualities that were once amusing are becoming irritating . </t>
@@ -8008,7 +8215,7 @@
     <t xml:space="preserve">a thriller without thrills and a mystery devoid of urgent questions . </t>
   </si>
   <si>
-    <t xml:space="preserve">a collage of clich�s and a dim echo of allusions to other films . </t>
+    <t xml:space="preserve">a collage of clich� and a dim echo of allusions to other films . </t>
   </si>
   <si>
     <t xml:space="preserve">the film is hampered by its predictable plot and paper-thin supporting characters . </t>
@@ -8050,7 +8257,22 @@
     <t xml:space="preserve">the whole thing's fairly lame , making it par for the course for disney sequels . </t>
   </si>
   <si>
-    <t xml:space="preserve">�its solemn pretension prevents us from sharing the awe in which it holds itself . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ts solemn pretension prevents us from sharing the awe in which it holds itself . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve"> . . . the good and different idea [of middle-aged romance] is not handled well and , except for the fine star performances , there is little else to recommend " never again . " </t>
@@ -8095,7 +8317,7 @@
     <t xml:space="preserve">less about shakespeare than the spawn of fools who saw quentin tarantino's handful of raucous gangster films and branched out into their own pseudo-witty copycat interpretations . </t>
   </si>
   <si>
-    <t xml:space="preserve">the film is like sitting in a downtown caf� , overhearing a bunch of typical late-twenty-somethings natter on about nothing , and desperately wishing you could change tables . </t>
+    <t xml:space="preserve">the film is like sitting in a downtown caf�, overhearing a bunch of typical late-twenty-somethings natter on about nothing , and desperately wishing you could change tables . </t>
   </si>
   <si>
     <t xml:space="preserve">this rather unfocused , all-over-the-map movie would be a lot better if it pared down its plots and characters to a few rather than dozens . . . or if it were subtler . . . or if it had a sense of humor . </t>
@@ -8207,7 +8429,7 @@
 while the transgressive trappings ( especially the frank sex scenes ) ensure that the film is never dull , rodrigues's beast-within metaphor is ultimately rather silly and overwrought , making the ambiguous ending seem goofy rather than provocative . 
 the satire is unfocused , while the story goes nowhere . 
 they threw loads of money at an idea that should've been so much more even if it was only made for teenage boys and wrestling fans . 
-it's mired in a shabby script that piles layer upon layer of action man clich� atop wooden dialogue and a shifting tone that falls far short of the peculiarly moral amorality of [woo's] best work . 
+it's mired in a shabby script that piles layer upon layer of action man clich�atop wooden dialogue and a shifting tone that falls far short of the peculiarly moral amorality of [woo's] best work . 
 reyes' directorial debut has good things to offer , but ultimately it's undone by a sloppy script
 if you're over 25 , have an iq over 90 , and have a driver's license , you should be able to find better entertainment . 
 the darker elements of misogyny and unprovoked violence suffocate the illumination created by the two daughters and the sparse instances of humor meant to shine through the gloomy film noir veil . 
@@ -8251,7 +8473,7 @@
     <t xml:space="preserve">due to stodgy , soap opera-ish dialogue , the rest of the cast comes across as stick figures reading lines from a teleprompter . </t>
   </si>
   <si>
-    <t xml:space="preserve">[t]he film is never sure to make a clear point � even if it seeks to rely on an ambiguous presentation . </t>
+    <t xml:space="preserve">[t]he film is never sure to make a clear point �even if it seeks to rely on an ambiguous presentation . </t>
   </si>
   <si>
     <t xml:space="preserve">while it may not add up to the sum of its parts , holofcener's film offers just enough insight to keep it from being simpleminded , and the ensemble cast is engaging enough to keep you from shifting in your chair too often . </t>
@@ -8629,7 +8851,7 @@
     <t xml:space="preserve">the problem with the mayhem in formula 51 is not that it's offensive , but that it's boring . </t>
   </si>
   <si>
-    <t xml:space="preserve">much of the digitally altered footage appears jagged , as if filmed directly from a television monitor , while the extensive use of stock footage quickly becomes a tiresome clich� . </t>
+    <t xml:space="preserve">much of the digitally altered footage appears jagged , as if filmed directly from a television monitor , while the extensive use of stock footage quickly becomes a tiresome clich�. </t>
   </si>
   <si>
     <t xml:space="preserve">the film never rises above a conventional , two dimension tale</t>
@@ -8701,7 +8923,7 @@
     <t xml:space="preserve">in the end , the movie bogs down in insignificance , saying nothing about kennedy's assassination and revealing nothing about the pathology it pretends to investigate . </t>
   </si>
   <si>
-    <t xml:space="preserve">starts out ballsy and stylish but fails to keep it up and settles into clich�s . </t>
+    <t xml:space="preserve">starts out ballsy and stylish but fails to keep it up and settles into clich� . </t>
   </si>
   <si>
     <t xml:space="preserve">sometimes makes less sense than the bruckheimeresque american action flicks it emulates . </t>
@@ -8725,7 +8947,7 @@
     <t xml:space="preserve">resident evil is what comes from taking john carpenter's ghosts of mars and eliminating the beheadings . in other words , about as bad a film you're likely to see all year . </t>
   </si>
   <si>
-    <t xml:space="preserve">five screenwriters are credited with the clich�-laden screenplay ; it seems as if each watered down the version of the one before . </t>
+    <t xml:space="preserve">five screenwriters are credited with the clich�laden screenplay ; it seems as if each watered down the version of the one before . </t>
   </si>
   <si>
     <t xml:space="preserve">the whole thing comes off like a particularly amateurish episode of bewitched that takes place during spring break . </t>
@@ -8740,7 +8962,7 @@
     <t xml:space="preserve">the movie's blatant derivativeness is one reason it's so lackluster . </t>
   </si>
   <si>
-    <t xml:space="preserve">la de salma es una versi�n de frida superficial , preciosista y sin ning�n contenido . </t>
+    <t xml:space="preserve">la de salma es una versi� de frida superficial , preciosista y sin ning� contenido . </t>
   </si>
   <si>
     <t xml:space="preserve">kids don't mind crappy movies as much as adults , provided there's lots of cute animals and clumsy people . 'snow dogs' has both . </t>
@@ -8755,7 +8977,7 @@
     <t xml:space="preserve">it's the humanizing stuff that will probably sink the film for anyone who doesn't think about percentages all day long . </t>
   </si>
   <si>
-    <t xml:space="preserve">ken russell would love this . in one scene , we get a stab at soccer hooliganism , a double-barreled rip-off of quentin tarantino's climactic shootout � and meat loaf explodes . </t>
+    <t xml:space="preserve">ken russell would love this . in one scene , we get a stab at soccer hooliganism , a double-barreled rip-off of quentin tarantino's climactic shootout �and meat loaf explodes . </t>
   </si>
   <si>
     <t xml:space="preserve">bella is the picture of health with boundless energy until a few days before she dies . this is absolutely and completely ridiculous and an insult to every family whose mother has suffered through the horrible pains of a death by cancer . </t>
@@ -8974,13 +9196,13 @@
     <t xml:space="preserve">what's missing in murder by numbers is any real psychological grounding for the teens' deviant behaviour . being latently gay and liking to read are hardly enough . </t>
   </si>
   <si>
-    <t xml:space="preserve">an uninspired preachy and clich�d war film . </t>
+    <t xml:space="preserve">an uninspired preachy and clich� war film . </t>
   </si>
   <si>
     <t xml:space="preserve">horrendously amateurish filmmaking that is plainly dull and visually ugly when it isn't incomprehensible . </t>
   </si>
   <si>
-    <t xml:space="preserve">a movie that harps on media-constructed 'issues' like whether compromise is the death of self� this orgasm [won't be an] exceedingly memorable one for most people . </t>
+    <t xml:space="preserve">a movie that harps on media-constructed 'issues' like whether compromise is the death of self�this orgasm [won't be an] exceedingly memorable one for most people . </t>
   </si>
   <si>
     <t xml:space="preserve">slackers' jokey approach to college education is disappointingly simplistic -- the film's biggest problem -- and there are no unforgettably stupid stunts or uproariously rude lines of dialogue to remember it by . </t>
@@ -9016,7 +9238,7 @@
     <t xml:space="preserve">sheridan's take on the author's schoolboy memoir . . . is a rather toothless take on a hard young life . </t>
   </si>
   <si>
-    <t xml:space="preserve">it jumps around with little logic or continuity , presenting backstage bytes of information that never amount to a satisfying complete picture of this particular , anciently demanding m�tier . </t>
+    <t xml:space="preserve">it jumps around with little logic or continuity , presenting backstage bytes of information that never amount to a satisfying complete picture of this particular , anciently demanding m�ier . </t>
   </si>
   <si>
     <t xml:space="preserve">how i killed my father is one of those art house films that makes you feel like you're watching an iceberg melt -- only it never melts . </t>
@@ -9109,7 +9331,7 @@
 the kind of film that leaves you scratching your head in amazement over the fact that so many talented people could participate in such an ill-advised and poorly executed idea . 
 nicks refuses to let slackers be seen as just another teen movie , which means he can be forgiven for frequently pandering to fans of the gross-out comedy . 
 nothing about the film -- with the possible exception of elizabeth hurley's breasts -- is authentic . 
-amid the clich� and foreshadowing , cage manages a degree of casual realism . . . that is routinely dynamited by blethyn . 
+amid the clich�and foreshadowing , cage manages a degree of casual realism . . . that is routinely dynamited by blethyn . 
 mostly , shafer and co-writer gregory hinton lack a strong-minded viewpoint , or a sense of humor . 
 no cliche escapes the perfervid treatment of gang warfare called ces wild . 
 eddie murphy and owen wilson have a cute partnership in i spy , but the movie around them is so often nearly nothing that their charm doesn't do a load of good . 
@@ -9177,7 +9399,7 @@
 the project's filmmakers forgot to include anything even halfway scary as they poorly rejigger fatal attraction into a high school setting . 
 in old-fashioned screenwriting parlance , ms . shreve's novel proved too difficult a text to 'lick , ' despite the efforts of a first-rate cast . 
 solondz may well be the only one laughing at his own joke
-stitch is a bad mannered , ugly and destructive little * * * * . no cute factor here� . not that i mind ugly ; the problem is he has no character , loveable or otherwise . 
+stitch is a bad mannered , ugly and destructive little * * * * . no cute factor here�. not that i mind ugly ; the problem is he has no character , loveable or otherwise . 
 deep down , i realized the harsh reality of my situation : i would leave the theater with a lower i . q . than when i had entered . 
 a really funny fifteen-minute short stretched beyond its limits to fill an almost feature-length film . 
 aside from the fact that the film idiotically uses the website feardotcom . com or the improperly hammy performance from poor stephen rea , the film gets added disdain for the fact that it is nearly impossible to look at or understand . 
@@ -9198,7 +9420,7 @@
 if deuces wild had been tweaked up a notch it would have become a camp adventure , one of those movies that's so bad it starts to become good . but it wasn't . 
 for a film about action , ultimate x is the gabbiest giant-screen movie ever , bogging down in a barrage of hype . 
  . . . a low rate annie featuring some kid who can't act , only echoes of jordan , and weirdo actor crispin glover screwing things up old school . 
-it might not be 1970s animation , but everything else about it is straight from the saturday morning cartoons � a retread story , bad writing , and the same old silliness . 
+it might not be 1970s animation , but everything else about it is straight from the saturday morning cartoons �a retread story , bad writing , and the same old silliness . 
 the picture seems uncertain whether it wants to be an acidic all-male all about eve or a lush , swooning melodrama in the intermezzo strain . 
 tends to plod . 
 a nearly 21/2 hours , the film is way too indulgent . 
@@ -9245,7 +9467,7 @@
     <t xml:space="preserve">tale will be all too familiar for anyone who's seen george roy hill's 1973 film , " the sting . " </t>
   </si>
   <si>
-    <t xml:space="preserve">gets the look and the period trappings right , but it otherwise drowns in a sea of visual and verbal clich�s . </t>
+    <t xml:space="preserve">gets the look and the period trappings right , but it otherwise drowns in a sea of visual and verbal clich� . </t>
   </si>
   <si>
     <t xml:space="preserve">it's hard to quibble with a flick boasting this many genuine cackles , but notorious c . h . o . still feels like a promising work-in-progress . </t>
@@ -9350,7 +9572,7 @@
     <t xml:space="preserve">as original and insightful as last week's episode of behind the music . </t>
   </si>
   <si>
-    <t xml:space="preserve">plays like john le carr� with a couple of burnt-out cylinders . </t>
+    <t xml:space="preserve">plays like john le carr�with a couple of burnt-out cylinders . </t>
   </si>
   <si>
     <t xml:space="preserve">you may be galled that you've wasted nearly two hours of your own precious life with this silly little puddle of a movie . </t>
@@ -9389,7 +9611,7 @@
     <t xml:space="preserve">the acting is just fine , but there's not enough substance here to sustain interest for the full 90 minutes , especially with the weak payoff . </t>
   </si>
   <si>
-    <t xml:space="preserve">after collateral damage , you might imagine that most every aggrieved father clich� has been unturned . but no . </t>
+    <t xml:space="preserve">after collateral damage , you might imagine that most every aggrieved father clich�has been unturned . but no . </t>
   </si>
   <si>
     <t xml:space="preserve">ultimately the , yes , snail-like pacing and lack of thematic resonance make the film more silly than scary , like some sort of martha stewart decorating program run amok . </t>
@@ -9509,7 +9731,7 @@
     <t xml:space="preserve">this low-rent -- and even lower-wit -- rip-off of the farrelly brothers' oeuvre gets way too mushy -- and in a relatively short amount of time . </t>
   </si>
   <si>
-    <t xml:space="preserve">it recycles every clich� about gays in what is essentially an extended soap opera . </t>
+    <t xml:space="preserve">it recycles every clich�about gays in what is essentially an extended soap opera . </t>
   </si>
   <si>
     <t xml:space="preserve">i'm all for the mentally challenged getting their fair shot in the movie business , but surely it doesn't have to be as a collection of keening and self-mutilating sideshow geeks . </t>
@@ -9638,7 +9860,30 @@
     <t xml:space="preserve">this pathetic junk is barely an hour long . nevertheless , it still seems endless . </t>
   </si>
   <si>
-    <t xml:space="preserve">it isn't that stealing harvard is a horrible movie�if only it were that grand a failure ! it's just that it's so not-at-all-good . and i expect much more from a talent as outstanding as director bruce mcculloch . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">it isn't that stealing harvard is a horrible movie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">뾦</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">f only it were that grand a failure ! it's just that it's so not-at-all-good . and i expect much more from a talent as outstanding as director bruce mcculloch . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">dolman confines himself to shtick and sentimentality -- the one bald and the other sloppy . </t>
@@ -9674,7 +9919,30 @@
     <t xml:space="preserve">the truth about charlie is that it's a brazenly misguided project . </t>
   </si>
   <si>
-    <t xml:space="preserve">caso voc� sinta necessidade de sair da sala antes do t�rmino da proje��o , n�o se preocupe : ningu�m lhe enviar� penas simbolizando covardia . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">caso voc�sinta necessidade de sair da sala antes do t�mino da proje</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">豫</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">o , n� se preocupe : ningu� lhe enviar�penas simbolizando covardia . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">displays the potential for a better movie than what bailly manages to deliver</t>
@@ -9986,7 +10254,7 @@
     <t xml:space="preserve">this painfully unfunny farce traffics in tired stereotypes and encumbers itself with complications . . . that have no bearing on the story . </t>
   </si>
   <si>
-    <t xml:space="preserve">short and sweet , but also more than anything else slight� tadpole pulls back from the consequences of its own actions and revelations . </t>
+    <t xml:space="preserve">short and sweet , but also more than anything else slight�tadpole pulls back from the consequences of its own actions and revelations . </t>
   </si>
   <si>
     <t xml:space="preserve">has its moments , but it's pretty far from a treasure . </t>
@@ -9998,7 +10266,30 @@
     <t xml:space="preserve">collateral damage offers formula payback and the big payoff , but the explosions tend to simply hit their marks , pyro-correctly . </t>
   </si>
   <si>
-    <t xml:space="preserve">the plan to make enough into �an inspiring tale of survival wrapped in the heart-pounding suspense of a stylish psychological thriller' has flopped as surely as a souffl� gone wrong . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">the plan to make enough into </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">멲</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">n inspiring tale of survival wrapped in the heart-pounding suspense of a stylish psychological thriller' has flopped as surely as a souffl�gone wrong . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">instead of letting the laughs come as they may , lawrence unleashes his trademark misogyny -- er , comedy -- like a human volcano or an overflowing septic tank , take your pick . </t>
@@ -10181,13 +10472,28 @@
     <t xml:space="preserve">all too familiar . . . basically the sort of cautionary tale that was old when 'angels with dirty faces' appeared in 1938 . </t>
   </si>
   <si>
-    <t xml:space="preserve">�passable enough for a shoot-out in the o . k . court house of life type of flick . strictly middle of the road . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿶</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">assable enough for a shoot-out in the o . k . court house of life type of flick . strictly middle of the road . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">although purportedly a study in modern alienation , it's really little more than a particularly slanted , gay s/m fantasy , enervating and deadeningly drawn-out . </t>
   </si>
   <si>
-    <t xml:space="preserve">after the first 10 minutes , which is worth seeing , the movie sinks into an abyss of clich�s , depression and bad alternative music . </t>
+    <t xml:space="preserve">after the first 10 minutes , which is worth seeing , the movie sinks into an abyss of clich� , depression and bad alternative music . </t>
   </si>
   <si>
     <t xml:space="preserve">no one can doubt the filmmakers' motives , but the guys still feels counterproductive . </t>
@@ -10210,7 +10516,7 @@
 disney again ransacks its archives for a quick-buck sequel . 
  coarse , cliched and clunky , this trifling romantic comedy in which opposites attract for no better reason than that the screenplay demands it squanders the charms of stars hugh grant and sandra bullock . 
 anyone who suffers through this film deserves , at the very least , a big box of consolation candy . 
-how much you are moved by the emotional tumult of [fran�ois and mich�le's] relationship depends a lot on how interesting and likable you find them . 
+how much you are moved by the emotional tumult of [fran�is and mich�e's] relationship depends a lot on how interesting and likable you find them . 
 they presume their audience won't sit still for a sociology lesson , however entertainingly presented , so they trot out the conventional science-fiction elements of bug-eyed monsters and futuristic women in skimpy clothes . 
 collapses after 30 minutes into a slap-happy series of adolescent violence . 
 the following things are not at all entertaining : the bad sound , the lack of climax and , worst of all , watching seinfeld ( who is also one of the film's producers ) do everything he can to look like a good guy . 
@@ -10224,7 +10530,7 @@
 a distinctly minor effort that will be seen to better advantage on cable , especially considering its barely feature-length running time of one hour . 
 most of the movie is so deadly dull that watching the proverbial paint dry would be a welcome improvement . 
 in the end , tuck everlasting falls victim to that everlasting conundrum experienced by every human who ever lived : too much to do , too little time to do it in . 
-rather less than the sum of its underventilated p�re-fils confrontations . 
+rather less than the sum of its underventilated p�e-fils confrontations . 
 mckay shows crushingly little curiosity about , or is ill-equipped to examine , the interior lives of the characters in his film , much less incorporate them into his narrative . 
 plays like a series of vignettes -- clips of a film that are still looking for a common through-line . 
 new yorkers always seem to find the oddest places to dwell . . . 
@@ -10244,7 +10550,7 @@
 for a film that celebrates radical , nonconformist values , what to do in case of fire ? lazily and glumly settles into a most traditional , reserved kind of filmmaking . 
 knockaround guys plays like a student film by two guys who desperately want to be quentin tarantino when they grow up . but they lack their idol's energy and passion for detail . 
 mattei so completely loses himself to the film's circular structure to ever offer any insightful discourse on , well , love in the time of money . 
-it briefly flirts with player masochism , but the point of real interest -� audience sadism -- is evaded completely . 
+it briefly flirts with player masochism , but the point of real interest -�audience sadism -- is evaded completely . 
 holland lets things peter out midway , but it's notably better acted -- and far less crass - than some other recent efforts in the burgeoning genre of films about black urban professionals . 
 for every articulate player , such as skateboarder tony hawk or bmx rider mat hoffman , are about a half dozen young turks angling to see how many times they can work the words " radical " or " suck " into a sentence . 
 there's not a fresh idea at the core of this tale . 
@@ -10278,7 +10584,7 @@
 frank capra played this story straight . but the 2002 film doesn't really believe in it , and breaks the mood with absurdly inappropriate 'comedy' scenes . 
 how about starting with a more original story instead of just slapping extreme humor and gross-out gags on top of the same old crap ? 
 the problem is that for the most part , the film is deadly dull . 
-handled correctly , wilde's play is a masterpiece of elegant wit and artifice . here , alas , it collapses like an overcooked souffl� . 
+handled correctly , wilde's play is a masterpiece of elegant wit and artifice . here , alas , it collapses like an overcooked souffl�. 
  " sorority boys " was funnier , and that movie was pretty bad . 
 a bizarre piece of work , with premise and dialogue at the level of kids' television and plot threads as morose as teen pregnancy , rape and suspected murder
 paul bettany is good at being the ultra-violent gangster wannabe , but the movie is certainly not number 1 . 
@@ -10476,7 +10782,30 @@
     <t xml:space="preserve">[a] stale retread of the '53 original . </t>
   </si>
   <si>
-    <t xml:space="preserve">one thing's for sure�if george romero had directed this movie , it wouldn't have taken the protagonists a full hour to determine that in order to kill a zombie you must shoot it in the head . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">one thing's for sure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">뾦</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">f george romero had directed this movie , it wouldn't have taken the protagonists a full hour to determine that in order to kill a zombie you must shoot it in the head . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">for dance completists only . </t>
@@ -10596,7 +10925,7 @@
     <t xml:space="preserve">it's not too fast and not too slow . it's not too racy and it's not too offensive . it's not too much of anything . </t>
   </si>
   <si>
-    <t xml:space="preserve">the great pity is that those responsible didn't cut their losses � and ours � and retitle it the adventures of direct-to-video nash , and send it to its proper home . </t>
+    <t xml:space="preserve">the great pity is that those responsible didn't cut their losses �and ours �and retitle it the adventures of direct-to-video nash , and send it to its proper home . </t>
   </si>
   <si>
     <t xml:space="preserve">about as original as a gangster sweating bullets while worrying about a contract on his life . </t>
@@ -10683,7 +11012,7 @@
     <t xml:space="preserve">the entire point of a shaggy dog story , of course , is that it goes nowhere , and this is classic nowheresville in every sense . </t>
   </si>
   <si>
-    <t xml:space="preserve">stale and clich�d to a fault . </t>
+    <t xml:space="preserve">stale and clich� to a fault . </t>
   </si>
   <si>
     <t xml:space="preserve">this film is too busy hitting all of its assigned marks to take on any life of its own . </t>
@@ -10737,7 +11066,7 @@
     <t xml:space="preserve">lacks the visual flair and bouncing bravado that characterizes better hip-hop clips and is content to recycle images and characters that were already tired 10 years ago . </t>
   </si>
   <si>
-    <t xml:space="preserve">'pocas ideas interesantes , un final pseudo m�stico que no corresponde al tono general del filme y que deja una sensaci�n de inconformidad que hace pensar m�s de una vez si vale la pena ir a la taquilla y reclamar el precio del boleto . '</t>
+    <t xml:space="preserve">'pocas ideas interesantes , un final pseudo m�tico que no corresponde al tono general del filme y que deja una sensaci� de inconformidad que hace pensar m� de una vez si vale la pena ir a la taquilla y reclamar el precio del boleto . '</t>
   </si>
   <si>
     <t xml:space="preserve">statham employs an accent that i think is supposed to be an attempt at hardass american but sometimes just lapses into unhidden british . </t>
@@ -10947,7 +11276,7 @@
     <t xml:space="preserve">[a] poorly executed comedy . </t>
   </si>
   <si>
-    <t xml:space="preserve">the movie's messages are quite admirable , but the story is just too clich�d and too often strains credulity . </t>
+    <t xml:space="preserve">the movie's messages are quite admirable , but the story is just too clich� and too often strains credulity . </t>
   </si>
   <si>
     <t xml:space="preserve">what we have here isn't a disaster , exactly , but a very handsomely produced let-down . </t>
@@ -11055,7 +11384,7 @@
     <t xml:space="preserve">it's definitely not made for kids or their parents , for that matter , and i think even fans of sandler's comic taste may find it uninteresting . </t>
   </si>
   <si>
-    <t xml:space="preserve">sheridan seems terrified of the book's irreverent energy , and scotches most of its �lan , humor , bile , and irony . </t>
+    <t xml:space="preserve">sheridan seems terrified of the book's irreverent energy , and scotches most of its �an , humor , bile , and irony . </t>
   </si>
   <si>
     <t xml:space="preserve">more busy than exciting , more frantic than involving , more chaotic than entertaining . </t>
@@ -11067,7 +11396,30 @@
     <t xml:space="preserve"> . . . really horrible drek . </t>
   </si>
   <si>
-    <t xml:space="preserve">it's as if solondz had two ideas for two movies , couldn't really figure out how to flesh either out , so he just slopped �em together here . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">it's as if solondz had two ideas for two movies , couldn't really figure out how to flesh either out , so he just slopped </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">멷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">m together here . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">the fourth in a series that i'll bet most parents had thought --hoped ! -- was a fad that had long since vanished . </t>
@@ -11256,7 +11608,7 @@
     <t xml:space="preserve">the densest distillation of roberts' movies ever made . </t>
   </si>
   <si>
-    <t xml:space="preserve">ultimately , the film never recovers from the clumsy clich� of the ugly american abroad , and the too-frosty exterior ms . paltrow employs to authenticate her british persona is another liability . </t>
+    <t xml:space="preserve">ultimately , the film never recovers from the clumsy clich�of the ugly american abroad , and the too-frosty exterior ms . paltrow employs to authenticate her british persona is another liability . </t>
   </si>
   <si>
     <t xml:space="preserve">a handsome but unfulfilling suspense drama more suited to a quiet evening on pbs than a night out at an amc . </t>
@@ -11469,7 +11821,7 @@
     <t xml:space="preserve">though its rather routine script is loaded with familiar situations , the movie has a cinematic fluidity and sense of intelligence that makes it work more than it probably should . </t>
   </si>
   <si>
-    <t xml:space="preserve"> one look at a girl in tight pants and big tits and you turn stupid ? " um� . . isn't that the basis for the entire plot ? 
+    <t xml:space="preserve"> one look at a girl in tight pants and big tits and you turn stupid ? " um�. . isn't that the basis for the entire plot ? 
  " not really as bad as you might think !  </t>
   </si>
   <si>
@@ -11626,7 +11978,30 @@
     <t xml:space="preserve">the master of disguise is awful . it's pauly shore awful . don't say you weren't warned . </t>
   </si>
   <si>
-    <t xml:space="preserve">disappointing in comparison to other recent war movies�or any other john woo flick for that matter . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">disappointing in comparison to other recent war movies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿵</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">r any other john woo flick for that matter . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">the entire movie is filled with deja vu moments . </t>
@@ -11734,7 +12109,7 @@
     <t xml:space="preserve">burns' fifth beer-soaked film feels in almost every possible way -- from the writing and direction to the soggy performances -- tossed off . </t>
   </si>
   <si>
-    <t xml:space="preserve">'es en verdad una pena que mandoki est� realizando cintas tan malas desde hace alg�n tiempo , pues talento tiene , pero qui�n sabe d�nde lo tiene escondido . '</t>
+    <t xml:space="preserve">'es en verdad una pena que mandoki est�realizando cintas tan malas desde hace alg� tiempo , pues talento tiene , pero qui� sabe d�de lo tiene escondido . '</t>
   </si>
   <si>
     <t xml:space="preserve">while this one gets off with a good natured warning , future lizard endeavors will need to adhere more closely to the laws of laughter</t>
@@ -11794,7 +12169,7 @@
     <t xml:space="preserve">death to smoochy tells a moldy-oldie , not-nearly -as-nasty -as-it- thinks-it-is joke . over and over again . </t>
   </si>
   <si>
-    <t xml:space="preserve">the threat implied in the title pok�mon 4ever is terrifying � like locusts in a horde these things will keep coming . </t>
+    <t xml:space="preserve">the threat implied in the title pok�on 4ever is terrifying �like locusts in a horde these things will keep coming . </t>
   </si>
   <si>
     <t xml:space="preserve">the film never gets over its own investment in conventional arrangements , in terms of love , age , gender , race , and class . </t>
@@ -11950,7 +12325,7 @@
     <t xml:space="preserve">one of the worst movies of the year . . . . watching it was painful . </t>
   </si>
   <si>
-    <t xml:space="preserve">a era do gelo diverte , mas n�o convence . � um passatempo descompromissado � e s� . </t>
+    <t xml:space="preserve">a era do gelo diverte , mas n� convence . �um passatempo descompromissado �e s�. </t>
   </si>
   <si>
     <t xml:space="preserve">no amount of burning , blasting , stabbing , and shooting can hide a weak script . </t>
@@ -11974,7 +12349,7 @@
     <t xml:space="preserve">the exploitative , clumsily staged violence overshadows everything , including most of the actors . </t>
   </si>
   <si>
-    <t xml:space="preserve">we started to wonder if � some unpaid intern had just typed 'chris rock , ' 'anthony hopkins' and 'terrorists' into some univac-like script machine . </t>
+    <t xml:space="preserve">we started to wonder if �some unpaid intern had just typed 'chris rock , ' 'anthony hopkins' and 'terrorists' into some univac-like script machine . </t>
   </si>
   <si>
     <t xml:space="preserve">even when crush departs from the 4w formula . . . it feels like a glossy rehash . </t>
@@ -11992,7 +12367,7 @@
     <t xml:space="preserve">this is very much of a mixed bag , with enough negatives to outweigh the positives . </t>
   </si>
   <si>
-    <t xml:space="preserve">marinated in clich�s and mawkish dialogue . </t>
+    <t xml:space="preserve">marinated in clich� and mawkish dialogue . </t>
   </si>
   <si>
     <t xml:space="preserve">whether it's the worst movie of 2002 , i can't say for sure : memories of rollerball have faded , and i skipped country bears . but this new jangle of noise , mayhem and stupidity must be a serious contender for the title . </t>
@@ -12094,7 +12469,7 @@
     <t xml:space="preserve">the result is so tame that even slightly wised-up kids would quickly change the channel . </t>
   </si>
   <si>
-    <t xml:space="preserve">it appears to have been modeled on the worst revenge-of-the-nerds clich�s the filmmakers could dredge up . </t>
+    <t xml:space="preserve">it appears to have been modeled on the worst revenge-of-the-nerds clich� the filmmakers could dredge up . </t>
   </si>
   <si>
     <t xml:space="preserve">nothing but an episode of smackdown ! in period costume and with a bigger budget . </t>
@@ -12115,7 +12490,7 @@
     <t xml:space="preserve">a tired , predictable , bordering on offensive , waste of time , money and celluloid . </t>
   </si>
   <si>
-    <t xml:space="preserve">if hill isn't quite his generation's don siegel ( or robert aldrich ) , it's because there's no discernible feeling beneath the chest hair ; it's all bluster and clich� . </t>
+    <t xml:space="preserve">if hill isn't quite his generation's don siegel ( or robert aldrich ) , it's because there's no discernible feeling beneath the chest hair ; it's all bluster and clich�. </t>
   </si>
   <si>
     <t xml:space="preserve">stealing harvard will dip into your wallet , swipe 90 minutes of your time , and offer you precisely this in recompense : a few early laughs scattered around a plot as thin as it is repetitious . </t>
@@ -12232,7 +12607,7 @@
     <t xml:space="preserve">a preposterously melodramatic paean to gang-member teens in brooklyn circa 1958 . </t>
   </si>
   <si>
-    <t xml:space="preserve">has none of the crackle of " fatal attraction " , " 9 � weeks " , or even " indecent proposal " , and feels more like lyne's stolid remake of " lolita " . </t>
+    <t xml:space="preserve">has none of the crackle of " fatal attraction " , " 9 �weeks " , or even " indecent proposal " , and feels more like lyne's stolid remake of " lolita " . </t>
   </si>
   <si>
     <t xml:space="preserve">everything its title implies , a standard-issue crime drama spat out from the tinseltown assembly line . </t>
@@ -12286,7 +12661,7 @@
     <t xml:space="preserve">this is a monumental achievement in practically every facet of inept filmmaking : joyless , idiotic , annoying , heavy-handed , visually atrocious , and often downright creepy . </t>
   </si>
   <si>
-    <t xml:space="preserve">this off-putting french romantic comedy is sure to test severely the indulgence of fans of am�lie . </t>
+    <t xml:space="preserve">this off-putting french romantic comedy is sure to test severely the indulgence of fans of am�ie . </t>
   </si>
   <si>
     <t xml:space="preserve">overburdened with complicated plotting and banal dialogue</t>
@@ -12406,7 +12781,7 @@
     <t xml:space="preserve">the filmmakers keep pushing the jokes at the expense of character until things fall apart . </t>
   </si>
   <si>
-    <t xml:space="preserve">rather than real figures , elling and kjell bjarne become symbolic characters whose actions are supposed to relate something about the na�f's encounter with the world . </t>
+    <t xml:space="preserve">rather than real figures , elling and kjell bjarne become symbolic characters whose actions are supposed to relate something about the na�'s encounter with the world . </t>
   </si>
   <si>
     <t xml:space="preserve">mariah carey gives us another peek at some of the magic we saw in glitter here in wisegirls . </t>
@@ -12481,7 +12856,22 @@
     <t xml:space="preserve">an awful movie that will only satisfy the most emotionally malleable of filmgoers . </t>
   </si>
   <si>
-    <t xml:space="preserve">�the story is far-flung , illogical , and plain stupid . </t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="WenQuanYi Micro Hei"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">꿻</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">he story is far-flung , illogical , and plain stupid . </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">the very simple story seems too simple and the working out of the plot almost arbitrary . </t>
@@ -12848,7 +13238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -12868,6 +13258,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="WenQuanYi Micro Hei"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -12912,8 +13307,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -12946,7 +13345,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="192.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="182.23"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -15321,7 +15720,7 @@
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="0" t="s">
+      <c r="A475" s="1" t="s">
         <v>474</v>
       </c>
     </row>
@@ -17956,7 +18355,7 @@
       </c>
     </row>
     <row r="1002" customFormat="false" ht="1569.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1002" s="1" t="s">
+      <c r="A1002" s="2" t="s">
         <v>1001</v>
       </c>
     </row>
@@ -18046,7 +18445,7 @@
       </c>
     </row>
     <row r="1020" customFormat="false" ht="1401.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1020" s="1" t="s">
+      <c r="A1020" s="2" t="s">
         <v>1019</v>
       </c>
     </row>
@@ -20286,7 +20685,7 @@
       </c>
     </row>
     <row r="1468" customFormat="false" ht="251.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1468" s="1" t="s">
+      <c r="A1468" s="2" t="s">
         <v>1467</v>
       </c>
     </row>
@@ -21386,7 +21785,7 @@
       </c>
     </row>
     <row r="1688" customFormat="false" ht="1972.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1688" s="1" t="s">
+      <c r="A1688" s="2" t="s">
         <v>1687</v>
       </c>
     </row>
@@ -21786,7 +22185,7 @@
       </c>
     </row>
     <row r="1768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1768" s="0" t="s">
+      <c r="A1768" s="1" t="s">
         <v>1767</v>
       </c>
     </row>
@@ -22446,7 +22845,7 @@
       </c>
     </row>
     <row r="1900" customFormat="false" ht="1259.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1900" s="1" t="s">
+      <c r="A1900" s="2" t="s">
         <v>1899</v>
       </c>
     </row>
@@ -23971,7 +24370,7 @@
       </c>
     </row>
     <row r="2205" customFormat="false" ht="426.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2205" s="1" t="s">
+      <c r="A2205" s="2" t="s">
         <v>2204</v>
       </c>
     </row>
@@ -24591,7 +24990,7 @@
       </c>
     </row>
     <row r="2329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2329" s="0" t="s">
+      <c r="A2329" s="1" t="s">
         <v>2328</v>
       </c>
     </row>
@@ -24811,7 +25210,7 @@
       </c>
     </row>
     <row r="2373" customFormat="false" ht="348.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2373" s="1" t="s">
+      <c r="A2373" s="2" t="s">
         <v>2372</v>
       </c>
     </row>
@@ -26281,7 +26680,7 @@
       </c>
     </row>
     <row r="2667" customFormat="false" ht="1636.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2667" s="1" t="s">
+      <c r="A2667" s="2" t="s">
         <v>2666</v>
       </c>
     </row>
@@ -27851,7 +28250,7 @@
       </c>
     </row>
     <row r="2981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2981" s="0" t="s">
+      <c r="A2981" s="1" t="s">
         <v>2980</v>
       </c>
     </row>
@@ -27881,7 +28280,7 @@
       </c>
     </row>
     <row r="2987" customFormat="false" ht="1636.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2987" s="1" t="s">
+      <c r="A2987" s="2" t="s">
         <v>2986</v>
       </c>
     </row>
@@ -29756,7 +30155,7 @@
       </c>
     </row>
     <row r="3362" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3362" s="1" t="s">
+      <c r="A3362" s="2" t="s">
         <v>3361</v>
       </c>
     </row>
@@ -31441,7 +31840,7 @@
       </c>
     </row>
     <row r="3699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3699" s="0" t="s">
+      <c r="A3699" s="1" t="s">
         <v>3698</v>
       </c>
     </row>

</xml_diff>